<commit_message>
Added MAPE (%) to the scoring
</commit_message>
<xml_diff>
--- a/Predictions/13/buckets.xlsx
+++ b/Predictions/13/buckets.xlsx
@@ -10,14 +10,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="KnAiQOwPpMaOiCVsmfgKr/DXunUQrY/C0uNELr7Je6o="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataChecksum="qygZhTHJwv0Hje7JJlPeFpNjgSBhaRyF4417uNQA+G8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>Lower</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>MAE</t>
+  </si>
+  <si>
+    <t>MAPE (%)</t>
   </si>
 </sst>
 </file>
@@ -85,14 +88,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -333,6 +335,9 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -344,7 +349,7 @@
       <c r="C2" s="2">
         <v>208808.3399</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>2134.0</v>
       </c>
       <c r="E2" s="2">
@@ -352,6 +357,9 @@
       </c>
       <c r="F2" s="2">
         <v>2844.152005134099</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.802343280922382</v>
       </c>
     </row>
     <row r="3">
@@ -364,7 +372,7 @@
       <c r="C3" s="2">
         <v>345675.9687999999</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>1635.0</v>
       </c>
       <c r="E3" s="2">
@@ -372,6 +380,9 @@
       </c>
       <c r="F3" s="2">
         <v>4806.00408711831</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.8153653754126</v>
       </c>
     </row>
     <row r="4">
@@ -384,7 +395,7 @@
       <c r="C4" s="2">
         <v>482543.5976999998</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>485.0</v>
       </c>
       <c r="E4" s="2">
@@ -392,6 +403,9 @@
       </c>
       <c r="F4" s="2">
         <v>6999.315103478812</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.71501472443991</v>
       </c>
     </row>
     <row r="5">
@@ -404,7 +418,7 @@
       <c r="C5" s="2">
         <v>619411.2265999997</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>269.0</v>
       </c>
       <c r="E5" s="2">
@@ -412,6 +426,9 @@
       </c>
       <c r="F5" s="2">
         <v>8987.823900495452</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.642655746809803</v>
       </c>
     </row>
     <row r="6">
@@ -424,7 +441,7 @@
       <c r="C6" s="2">
         <v>756278.8554999996</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>118.0</v>
       </c>
       <c r="E6" s="2">
@@ -432,6 +449,9 @@
       </c>
       <c r="F6" s="2">
         <v>13374.08757157236</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.922819891986461</v>
       </c>
     </row>
     <row r="7">
@@ -444,7 +464,7 @@
       <c r="C7" s="2">
         <v>893146.4843999996</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>53.0</v>
       </c>
       <c r="E7" s="2">
@@ -452,6 +472,9 @@
       </c>
       <c r="F7" s="2">
         <v>13986.47701815339</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.685913917965953</v>
       </c>
     </row>
     <row r="8">
@@ -464,7 +487,7 @@
       <c r="C8" s="2">
         <v>1030014.1133</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>21.0</v>
       </c>
       <c r="E8" s="2">
@@ -472,6 +495,9 @@
       </c>
       <c r="F8" s="2">
         <v>13537.08711843789</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.399112572210758</v>
       </c>
     </row>
     <row r="9">
@@ -484,7 +510,7 @@
       <c r="C9" s="2">
         <v>1166881.7422</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>17.0</v>
       </c>
       <c r="E9" s="2">
@@ -492,6 +518,9 @@
       </c>
       <c r="F9" s="2">
         <v>23721.49441253347</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2.181915387043861</v>
       </c>
     </row>
     <row r="10">
@@ -504,7 +533,7 @@
       <c r="C10" s="2">
         <v>1303749.371099999</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>11.0</v>
       </c>
       <c r="E10" s="2">
@@ -512,6 +541,9 @@
       </c>
       <c r="F10" s="2">
         <v>17029.94258946157</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.379172410107623</v>
       </c>
     </row>
     <row r="11">
@@ -524,7 +556,7 @@
       <c r="C11" s="2">
         <v>1440616.999999999</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>20.0</v>
       </c>
       <c r="E11" s="2">
@@ -532,6 +564,9 @@
       </c>
       <c r="F11" s="2">
         <v>19663.44570702263</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.420271646561696</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1551,6 +1586,9 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -1562,7 +1600,7 @@
       <c r="C2" s="2">
         <v>213231.2769</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>3006.0</v>
       </c>
       <c r="E2" s="2">
@@ -1570,6 +1608,9 @@
       </c>
       <c r="F2" s="2">
         <v>2856.185104105414</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.802948896516745</v>
       </c>
     </row>
     <row r="3">
@@ -1582,7 +1623,7 @@
       <c r="C3" s="2">
         <v>354654.4127999999</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>2196.0</v>
       </c>
       <c r="E3" s="2">
@@ -1590,6 +1631,9 @@
       </c>
       <c r="F3" s="2">
         <v>4893.083239211453</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.830549650835914</v>
       </c>
     </row>
     <row r="4">
@@ -1602,7 +1646,7 @@
       <c r="C4" s="2">
         <v>496077.5486999999</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>673.0</v>
       </c>
       <c r="E4" s="2">
@@ -1610,6 +1654,9 @@
       </c>
       <c r="F4" s="2">
         <v>7070.476054070927</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.658337069468952</v>
       </c>
     </row>
     <row r="5">
@@ -1622,7 +1669,7 @@
       <c r="C5" s="2">
         <v>637500.6845999999</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>320.0</v>
       </c>
       <c r="E5" s="2">
@@ -1630,6 +1677,9 @@
       </c>
       <c r="F5" s="2">
         <v>8259.94324729009</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.48284283754976</v>
       </c>
     </row>
     <row r="6">
@@ -1642,7 +1692,7 @@
       <c r="C6" s="2">
         <v>778923.8204999999</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>177.0</v>
       </c>
       <c r="E6" s="2">
@@ -1650,6 +1700,9 @@
       </c>
       <c r="F6" s="2">
         <v>9937.244230179509</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.424327628293317</v>
       </c>
     </row>
     <row r="7">
@@ -1662,7 +1715,7 @@
       <c r="C7" s="2">
         <v>920346.9563999999</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>75.0</v>
       </c>
       <c r="E7" s="2">
@@ -1670,6 +1723,9 @@
       </c>
       <c r="F7" s="2">
         <v>14854.79399876518</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.771607214676779</v>
       </c>
     </row>
     <row r="8">
@@ -1682,7 +1738,7 @@
       <c r="C8" s="2">
         <v>1061770.0923</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>67.0</v>
       </c>
       <c r="E8" s="2">
@@ -1690,6 +1746,9 @@
       </c>
       <c r="F8" s="2">
         <v>14656.46048676774</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1.449610974414076</v>
       </c>
     </row>
     <row r="9">
@@ -1702,7 +1761,7 @@
       <c r="C9" s="2">
         <v>1203193.2282</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>20.0</v>
       </c>
       <c r="E9" s="2">
@@ -1710,6 +1769,9 @@
       </c>
       <c r="F9" s="2">
         <v>16519.76196206952</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.455178917219898</v>
       </c>
     </row>
     <row r="10">
@@ -1722,7 +1784,7 @@
       <c r="C10" s="2">
         <v>1344616.3641</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>30.0</v>
       </c>
       <c r="E10" s="2">
@@ -1730,6 +1792,9 @@
       </c>
       <c r="F10" s="2">
         <v>20457.47702179259</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.580982976561259</v>
       </c>
     </row>
     <row r="11">
@@ -1742,7 +1807,7 @@
       <c r="C11" s="2">
         <v>1486039.5</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>29.0</v>
       </c>
       <c r="E11" s="2">
@@ -1750,6 +1815,9 @@
       </c>
       <c r="F11" s="2">
         <v>20588.25636983541</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.459964673323734</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>